<commit_message>
R Community final version
</commit_message>
<xml_diff>
--- a/Data/population data.xlsx
+++ b/Data/population data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{0FF2DE82-B7F6-45B9-863C-BC95D955DE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF2CA249-E23F-4763-806A-A060B766EC98}"/>
+    <workbookView xWindow="-14400" yWindow="-375" windowWidth="14400" windowHeight="15600" xr2:uid="{BF2CA249-E23F-4763-806A-A060B766EC98}"/>
   </bookViews>
   <sheets>
     <sheet name="district" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -470,22 +470,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -826,32 +820,32 @@
   <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="15">
+      <c r="C1" s="13">
         <v>2018</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>2020</v>
       </c>
-      <c r="E1" s="15">
+      <c r="E1" s="13">
         <v>2021</v>
       </c>
-      <c r="F1" s="15">
+      <c r="F1" s="13">
         <v>2022</v>
       </c>
     </row>
@@ -2467,351 +2461,351 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="13">
+      <c r="B1" s="11">
         <v>2018</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="12">
         <v>2020</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="12">
         <v>2021</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="12">
         <v>2022</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>185800</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>194600</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>198900</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>201500</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>1654800</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>1714200</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>1704100</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>1695200</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>475600</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>500100</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>508400</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>513800</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>320800</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>339200</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>344000</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>347700</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>49500</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>51400</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>51800</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>52100</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>172400</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>180000</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>181800</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>182700</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <v>121200</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>125200</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>126500</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>127300</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>247500</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>254600</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>256800</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>258200</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>525900</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>542100</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>543700</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>543500</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>54000</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>57300</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>58100</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>58700</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>52700</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>54900</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>54700</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>54500</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>48700</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>51300</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>51600</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>51900</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>32400</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>32800</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>32900</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>32700</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>622800</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>644000</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>650200</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>655000</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>235000</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>245000</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>244600</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>246000</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>100500</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>102800</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>102500</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>102400</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>3753700</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>3901300</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>3916000</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>3922000</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>1146200</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>1188100</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>1194600</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>1201300</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>4900600</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>5090200</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>5111400</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>5124100</v>
       </c>
     </row>

</xml_diff>